<commit_message>
Fix classes for some drivers.
</commit_message>
<xml_diff>
--- a/2019/cvscc-20190623.xlsx
+++ b/2019/cvscc-20190623.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jrye/personal/mac/results/2019/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B47A9ED-F19A-D141-A108-F7511844B908}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34072363-8C91-C448-B989-BD5722ECF144}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1080" yWindow="460" windowWidth="23500" windowHeight="19460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1622" uniqueCount="564">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1622" uniqueCount="565">
   <si>
     <t>Run Order</t>
   </si>
@@ -1723,13 +1723,16 @@
   </si>
   <si>
     <t>CAMC</t>
+  </si>
+  <si>
+    <t>CAMT</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1790,6 +1793,12 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -1835,7 +1844,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -1858,6 +1867,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2175,7 +2185,7 @@
   <dimension ref="A1:AC998"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18:D19"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -3052,8 +3062,8 @@
         <v>415</v>
       </c>
       <c r="C17"/>
-      <c r="D17" t="s">
-        <v>562</v>
+      <c r="D17" s="16" t="s">
+        <v>564</v>
       </c>
       <c r="E17" t="s">
         <v>416</v>
@@ -3115,8 +3125,8 @@
         <v>418</v>
       </c>
       <c r="C18"/>
-      <c r="D18" t="s">
-        <v>562</v>
+      <c r="D18" s="16" t="s">
+        <v>564</v>
       </c>
       <c r="E18" t="s">
         <v>416</v>
@@ -3178,8 +3188,8 @@
         <v>420</v>
       </c>
       <c r="C19"/>
-      <c r="D19" t="s">
-        <v>562</v>
+      <c r="D19" s="16" t="s">
+        <v>564</v>
       </c>
       <c r="E19" t="s">
         <v>416</v>
@@ -10447,7 +10457,7 @@
         <v>0.8</v>
       </c>
       <c r="K34">
-        <f t="shared" ref="K34:K65" si="1">J34*L34</f>
+        <f t="shared" ref="K34:K64" si="1">J34*L34</f>
         <v>50.42</v>
       </c>
       <c r="L34">

</xml_diff>